<commit_message>
#48 add pagination in lessstock table done
</commit_message>
<xml_diff>
--- a/public/Product Report.xlsx
+++ b/public/Product Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Title</t>
   </si>
@@ -30,18 +30,6 @@
   </si>
   <si>
     <t>Envoice No</t>
-  </si>
-  <si>
-    <t>sample product</t>
-  </si>
-  <si>
-    <t>2023-06-19</t>
-  </si>
-  <si>
-    <t>batch 1</t>
-  </si>
-  <si>
-    <t>L160620239</t>
   </si>
 </sst>
 </file>
@@ -381,7 +369,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,23 +394,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>